<commit_message>
Update E6 HR Data - Sorting and Filtering.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/Exercise 6/E6 HR Data - Sorting and Filtering.xlsx
+++ b/Exercise Files/Exercise 6/E6 HR Data - Sorting and Filtering.xlsx
@@ -1,33 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f21e54c367d3358c/Documents/01 Work Files/05 SSIT/Online Courses/Advanced PivotTables/Exercise Files/Exercise 6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wayvy Technologies\Documents\GitHub\PivotTables\Exercise Files\Exercise 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{F6E5A937-8454-4ED5-A4B5-E29ED65969AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5FF920D9-AB71-4EAC-95FC-0DC11000A733}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F6D0BE-F7AF-4FA9-8551-5B727CAC2C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Employee Salary" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="Employee Info" sheetId="1" r:id="rId2"/>
+    <sheet name="Employee Salary" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Employee Salary'!$A$3:$B$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$B$25</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable11" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable21" hidden="1">'[1]Department Info'!$A$1:$A$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[1]Job Info'!$A$1:$A$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[2]Job Info'!$A$1:$A$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -100,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="129">
   <si>
     <t>Employee ID</t>
   </si>
@@ -484,6 +488,9 @@
   </si>
   <si>
     <t xml:space="preserve">Salary </t>
+  </si>
+  <si>
+    <t>Sum of Salary</t>
   </si>
 </sst>
 </file>
@@ -642,15 +649,26 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Department Info"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="Job Info"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1799,8 +1817,245 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{413CF33D-1EBB-40D4-BD22-1E329711258E}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" customListSort="0">
-  <location ref="A3:B110" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{70A20ECE-C92A-48B2-9B29-9B8E80E4152C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="100">
+        <item x="22"/>
+        <item x="87"/>
+        <item x="31"/>
+        <item x="54"/>
+        <item x="56"/>
+        <item x="59"/>
+        <item x="82"/>
+        <item x="30"/>
+        <item x="92"/>
+        <item x="84"/>
+        <item x="18"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="6"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="74"/>
+        <item x="67"/>
+        <item x="4"/>
+        <item x="86"/>
+        <item x="63"/>
+        <item x="12"/>
+        <item x="81"/>
+        <item x="20"/>
+        <item x="71"/>
+        <item x="65"/>
+        <item x="85"/>
+        <item x="70"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="93"/>
+        <item x="37"/>
+        <item x="13"/>
+        <item x="69"/>
+        <item x="47"/>
+        <item x="95"/>
+        <item x="50"/>
+        <item x="14"/>
+        <item x="44"/>
+        <item x="43"/>
+        <item x="88"/>
+        <item x="60"/>
+        <item x="97"/>
+        <item x="32"/>
+        <item x="79"/>
+        <item x="29"/>
+        <item x="21"/>
+        <item x="98"/>
+        <item x="40"/>
+        <item x="49"/>
+        <item x="90"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="38"/>
+        <item x="94"/>
+        <item x="57"/>
+        <item x="75"/>
+        <item x="80"/>
+        <item x="5"/>
+        <item x="26"/>
+        <item x="55"/>
+        <item x="48"/>
+        <item x="35"/>
+        <item x="7"/>
+        <item x="52"/>
+        <item x="36"/>
+        <item x="91"/>
+        <item x="89"/>
+        <item x="39"/>
+        <item x="8"/>
+        <item x="62"/>
+        <item x="23"/>
+        <item x="28"/>
+        <item x="64"/>
+        <item x="96"/>
+        <item x="34"/>
+        <item x="73"/>
+        <item x="51"/>
+        <item x="33"/>
+        <item x="61"/>
+        <item x="27"/>
+        <item x="17"/>
+        <item x="46"/>
+        <item x="58"/>
+        <item x="15"/>
+        <item x="72"/>
+        <item x="16"/>
+        <item x="76"/>
+        <item x="3"/>
+        <item x="77"/>
+        <item x="9"/>
+        <item x="66"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="78"/>
+        <item x="53"/>
+        <item x="45"/>
+        <item x="68"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="22">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Salary" fld="5" baseField="1" baseItem="4" numFmtId="42"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="1" type="captionBeginsWith" evalOrder="-1" id="1" stringValue1="A">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter val="A*"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{413CF33D-1EBB-40D4-BD22-1E329711258E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" customListSort="0">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -1920,12 +2175,12 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="8">
         <item x="0"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="6"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="2"/>
+        <item h="1" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1938,7 +2193,7 @@
     <field x="3"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="107">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -1946,316 +2201,16 @@
       <x v="9"/>
     </i>
     <i r="1">
-      <x v="37"/>
-    </i>
-    <i r="1">
       <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="49"/>
     </i>
     <i r="1">
       <x v="12"/>
     </i>
     <i r="1">
-      <x v="32"/>
-    </i>
-    <i r="1">
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="89"/>
-    </i>
-    <i r="1">
-      <x v="56"/>
-    </i>
-    <i r="1">
-      <x v="27"/>
-    </i>
-    <i r="1">
-      <x v="62"/>
-    </i>
-    <i r="1">
-      <x v="72"/>
-    </i>
-    <i r="1">
-      <x v="66"/>
-    </i>
-    <i r="1">
-      <x v="63"/>
-    </i>
-    <i r="1">
-      <x v="33"/>
-    </i>
-    <i r="1">
-      <x v="97"/>
-    </i>
-    <i r="1">
       <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="73"/>
-    </i>
-    <i r="1">
-      <x v="65"/>
-    </i>
-    <i r="1">
-      <x v="36"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="45"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i r="1">
-      <x v="94"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="39"/>
-    </i>
-    <i r="1">
-      <x v="26"/>
-    </i>
-    <i r="1">
-      <x v="55"/>
-    </i>
-    <i r="1">
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="82"/>
-    </i>
-    <i r="1">
-      <x v="47"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="40"/>
-    </i>
-    <i r="1">
-      <x v="68"/>
-    </i>
-    <i r="1">
-      <x v="43"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="95"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="41"/>
-    </i>
-    <i r="1">
-      <x v="92"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="74"/>
-    </i>
-    <i r="1">
-      <x v="42"/>
-    </i>
-    <i r="1">
-      <x v="35"/>
-    </i>
-    <i r="1">
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="57"/>
-    </i>
-    <i r="1">
-      <x v="54"/>
-    </i>
-    <i r="1">
-      <x v="64"/>
-    </i>
-    <i r="1">
-      <x v="76"/>
-    </i>
-    <i r="1">
-      <x v="93"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i r="1">
-      <x v="53"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="81"/>
-    </i>
-    <i r="1">
-      <x v="91"/>
-    </i>
-    <i r="1">
-      <x v="96"/>
-    </i>
-    <i r="1">
-      <x v="88"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="75"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="70"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="60"/>
-    </i>
-    <i r="1">
-      <x v="61"/>
-    </i>
-    <i r="1">
-      <x v="80"/>
-    </i>
-    <i r="1">
-      <x v="50"/>
-    </i>
-    <i r="1">
-      <x v="31"/>
-    </i>
-    <i r="1">
-      <x v="87"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="29"/>
-    </i>
-    <i r="1">
-      <x v="71"/>
-    </i>
-    <i r="1">
-      <x v="86"/>
-    </i>
-    <i r="1">
-      <x v="83"/>
-    </i>
-    <i r="1">
-      <x v="85"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
-    </i>
-    <i r="1">
-      <x v="58"/>
-    </i>
-    <i r="1">
-      <x v="84"/>
-    </i>
-    <i r="1">
-      <x v="44"/>
-    </i>
-    <i r="1">
-      <x v="69"/>
-    </i>
-    <i r="1">
-      <x v="46"/>
-    </i>
-    <i r="1">
-      <x v="25"/>
-    </i>
-    <i r="1">
-      <x v="38"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="98"/>
-    </i>
-    <i r="1">
-      <x v="77"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="90"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="67"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="79"/>
-    </i>
-    <i r="1">
-      <x v="59"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="34"/>
-    </i>
-    <i r="1">
-      <x v="48"/>
-    </i>
-    <i r="1">
-      <x v="78"/>
     </i>
     <i t="grand">
       <x/>
@@ -2268,6 +2223,17 @@
     <dataField name="Salary " fld="5" baseField="1" baseItem="1" numFmtId="42"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="1" type="captionBeginsWith" evalOrder="-1" id="1" stringValue1="A">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter val="A*"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -2297,9 +2263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2337,7 +2303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2443,7 +2409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2585,33 +2551,268 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACDC970-2C3B-474F-96A3-D147F7725AC9}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A3:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="5">
+        <v>397828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5">
+        <v>99568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="5">
+        <v>94050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5">
+        <v>86734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="5">
+        <v>79270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="5">
+        <v>38206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="5">
+        <v>126231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="5">
+        <v>70085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="5">
+        <v>56146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="5">
+        <v>47852</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5">
+        <v>47852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="5">
+        <v>89653</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5">
+        <v>61939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="5">
+        <v>27714</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="5">
+        <v>123718</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5">
+        <v>71398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5">
+        <v>52320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="5">
+        <v>43304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="5">
+        <v>43304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="5">
+        <v>85983</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="5">
+        <v>85983</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="5">
+        <v>914569</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:B25" xr:uid="{8ACDC970-2C3B-474F-96A3-D147F7725AC9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Aden Salazar"/>
+        <filter val="Aiden Oconnell"/>
+        <filter val="Alanna Ochoa"/>
+        <filter val="Alena Arnold"/>
+        <filter val="Alisa Davies"/>
+        <filter val="Alma Dean"/>
+        <filter val="Amaris Waters"/>
+        <filter val="Amber Austin"/>
+        <filter val="Anabella Anderson"/>
+        <filter val="Anya Anderson"/>
+        <filter val="Areli Cooke"/>
+        <filter val="Ashleigh Chung"/>
+        <filter val="Ayanna Maldonado"/>
+        <filter val="Aydan Roy"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="$70,085"/>
+        <filter val="$71,398"/>
+        <filter val="$79,270"/>
+        <filter val="$85,983"/>
+        <filter val="$86,734"/>
+        <filter val="$94,050"/>
+        <filter val="$99,568"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91CF34E-7D4C-4202-8C48-E09665776E8A}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2838,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2100</v>
       </c>
@@ -2663,7 +2864,7 @@
         <v>40445</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2101</v>
       </c>
@@ -2689,7 +2890,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2102</v>
       </c>
@@ -2715,7 +2916,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -2741,7 +2942,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2104</v>
       </c>
@@ -2767,7 +2968,7 @@
         <v>40164</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2105</v>
       </c>
@@ -2793,7 +2994,7 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2106</v>
       </c>
@@ -2819,7 +3020,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2107</v>
       </c>
@@ -2845,7 +3046,7 @@
         <v>38555</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2108</v>
       </c>
@@ -2871,7 +3072,7 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2109</v>
       </c>
@@ -2897,7 +3098,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2110</v>
       </c>
@@ -2923,7 +3124,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2111</v>
       </c>
@@ -2949,7 +3150,7 @@
         <v>40378</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2112</v>
       </c>
@@ -2975,7 +3176,7 @@
         <v>40976</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2113</v>
       </c>
@@ -3001,7 +3202,7 @@
         <v>36845</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2114</v>
       </c>
@@ -3027,7 +3228,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2115</v>
       </c>
@@ -3053,7 +3254,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2116</v>
       </c>
@@ -3079,7 +3280,7 @@
         <v>36704</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2117</v>
       </c>
@@ -3105,7 +3306,7 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2118</v>
       </c>
@@ -3131,7 +3332,7 @@
         <v>41286</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2119</v>
       </c>
@@ -3157,7 +3358,7 @@
         <v>39319</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2120</v>
       </c>
@@ -3183,7 +3384,7 @@
         <v>40839</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2121</v>
       </c>
@@ -3209,7 +3410,7 @@
         <v>36754</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2122</v>
       </c>
@@ -3235,7 +3436,7 @@
         <v>38170</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2123</v>
       </c>
@@ -3261,7 +3462,7 @@
         <v>39164</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2124</v>
       </c>
@@ -3287,7 +3488,7 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2125</v>
       </c>
@@ -3313,7 +3514,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2126</v>
       </c>
@@ -3339,7 +3540,7 @@
         <v>41065</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2127</v>
       </c>
@@ -3365,7 +3566,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2128</v>
       </c>
@@ -3391,7 +3592,7 @@
         <v>42030</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2129</v>
       </c>
@@ -3417,7 +3618,7 @@
         <v>39499</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2130</v>
       </c>
@@ -3443,7 +3644,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2131</v>
       </c>
@@ -3469,7 +3670,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2132</v>
       </c>
@@ -3495,7 +3696,7 @@
         <v>36600</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2133</v>
       </c>
@@ -3521,7 +3722,7 @@
         <v>39803</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2134</v>
       </c>
@@ -3547,7 +3748,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2135</v>
       </c>
@@ -3573,7 +3774,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2136</v>
       </c>
@@ -3599,7 +3800,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2137</v>
       </c>
@@ -3625,7 +3826,7 @@
         <v>38241</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2138</v>
       </c>
@@ -3651,7 +3852,7 @@
         <v>40684</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2139</v>
       </c>
@@ -3677,7 +3878,7 @@
         <v>39996</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2140</v>
       </c>
@@ -3703,7 +3904,7 @@
         <v>37411</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2141</v>
       </c>
@@ -3729,7 +3930,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2142</v>
       </c>
@@ -3755,7 +3956,7 @@
         <v>43170</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2143</v>
       </c>
@@ -3781,7 +3982,7 @@
         <v>37292</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2144</v>
       </c>
@@ -3807,7 +4008,7 @@
         <v>37609</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2145</v>
       </c>
@@ -3833,7 +4034,7 @@
         <v>37094</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2146</v>
       </c>
@@ -3859,7 +4060,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2147</v>
       </c>
@@ -3885,7 +4086,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2148</v>
       </c>
@@ -3911,7 +4112,7 @@
         <v>38742</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2149</v>
       </c>
@@ -3937,7 +4138,7 @@
         <v>40047</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2150</v>
       </c>
@@ -3963,7 +4164,7 @@
         <v>39802</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2151</v>
       </c>
@@ -3989,7 +4190,7 @@
         <v>39616</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2152</v>
       </c>
@@ -4015,7 +4216,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2153</v>
       </c>
@@ -4041,7 +4242,7 @@
         <v>39019</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2154</v>
       </c>
@@ -4067,7 +4268,7 @@
         <v>41028</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2155</v>
       </c>
@@ -4093,7 +4294,7 @@
         <v>39768</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2156</v>
       </c>
@@ -4119,7 +4320,7 @@
         <v>41153</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2157</v>
       </c>
@@ -4145,7 +4346,7 @@
         <v>36847</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2158</v>
       </c>
@@ -4171,7 +4372,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2159</v>
       </c>
@@ -4197,7 +4398,7 @@
         <v>39744</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2160</v>
       </c>
@@ -4223,7 +4424,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2161</v>
       </c>
@@ -4249,7 +4450,7 @@
         <v>38401</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2162</v>
       </c>
@@ -4275,7 +4476,7 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2163</v>
       </c>
@@ -4301,7 +4502,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2164</v>
       </c>
@@ -4327,7 +4528,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2165</v>
       </c>
@@ -4353,7 +4554,7 @@
         <v>39740</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2166</v>
       </c>
@@ -4379,7 +4580,7 @@
         <v>40408</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2167</v>
       </c>
@@ -4405,7 +4606,7 @@
         <v>38822</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2168</v>
       </c>
@@ -4431,7 +4632,7 @@
         <v>40083</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2169</v>
       </c>
@@ -4457,7 +4658,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2170</v>
       </c>
@@ -4483,7 +4684,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2171</v>
       </c>
@@ -4509,7 +4710,7 @@
         <v>41582</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2172</v>
       </c>
@@ -4535,7 +4736,7 @@
         <v>36663</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2173</v>
       </c>
@@ -4561,7 +4762,7 @@
         <v>37526</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2174</v>
       </c>
@@ -4587,7 +4788,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2175</v>
       </c>
@@ -4613,7 +4814,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2176</v>
       </c>
@@ -4639,7 +4840,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2177</v>
       </c>
@@ -4665,7 +4866,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2178</v>
       </c>
@@ -4691,7 +4892,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2179</v>
       </c>
@@ -4717,7 +4918,7 @@
         <v>42462</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2180</v>
       </c>
@@ -4743,7 +4944,7 @@
         <v>41654</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2181</v>
       </c>
@@ -4769,7 +4970,7 @@
         <v>43128</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2182</v>
       </c>
@@ -4795,7 +4996,7 @@
         <v>43381</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2183</v>
       </c>
@@ -4821,7 +5022,7 @@
         <v>41676</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2184</v>
       </c>
@@ -4847,7 +5048,7 @@
         <v>36651</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2185</v>
       </c>
@@ -4873,7 +5074,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2186</v>
       </c>
@@ -4899,7 +5100,7 @@
         <v>38565</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2187</v>
       </c>
@@ -4925,7 +5126,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2188</v>
       </c>
@@ -4951,7 +5152,7 @@
         <v>39656</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2189</v>
       </c>
@@ -4977,7 +5178,7 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2190</v>
       </c>
@@ -5003,7 +5204,7 @@
         <v>42528</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2191</v>
       </c>
@@ -5029,7 +5230,7 @@
         <v>38499</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2192</v>
       </c>
@@ -5055,7 +5256,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2193</v>
       </c>
@@ -5081,7 +5282,7 @@
         <v>38384</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2194</v>
       </c>
@@ -5107,7 +5308,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2195</v>
       </c>
@@ -5133,7 +5334,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2196</v>
       </c>
@@ -5159,7 +5360,7 @@
         <v>37442</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2197</v>
       </c>
@@ -5185,7 +5386,7 @@
         <v>38690</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2198</v>
       </c>
@@ -5219,28 +5420,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8EEB18-62AF-48A5-8FC5-BF1CEC0909F8}">
-  <dimension ref="A3:B110"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
@@ -5248,15 +5450,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="5">
-        <v>1258435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>397828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>87</v>
       </c>
@@ -5264,847 +5466,58 @@
         <v>99568</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5">
-        <v>95191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5">
-        <v>94050</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>86734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B8" s="5">
-        <v>87377</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>79270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5">
-        <v>86734</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>3</v>
+        <v>38206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="B10" s="5">
-        <v>86135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="5">
-        <v>79270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="5">
-        <v>78844</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="5">
-        <v>76212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="5">
-        <v>71067</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="5">
-        <v>61955</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="5">
-        <v>61590</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="5">
-        <v>58190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="5">
-        <v>52949</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="5">
-        <v>50831</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="5">
-        <v>48094</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="5">
-        <v>38206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="5">
-        <v>32172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="5">
-        <v>699842</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="5">
-        <v>86357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5">
-        <v>83169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="5">
-        <v>70918</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="5">
-        <v>70085</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="5">
-        <v>63662</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="5">
-        <v>57759</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="5">
-        <v>56445</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="5">
-        <v>56146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="5">
-        <v>47199</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="5">
-        <v>44737</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="5">
-        <v>33778</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="5">
-        <v>29587</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="5">
-        <v>1079786</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="5">
-        <v>99248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="5">
-        <v>97719</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="5">
-        <v>85288</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="5">
-        <v>84859</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="5">
-        <v>79980</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="5">
-        <v>78694</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="5">
-        <v>72568</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="5">
-        <v>66314</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="5">
-        <v>64872</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="5">
-        <v>63016</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="5">
-        <v>55197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="5">
-        <v>55175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="5">
-        <v>47852</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="5">
-        <v>40979</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="5">
-        <v>33900</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="5">
-        <v>27723</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="5">
-        <v>26402</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="5">
-        <v>903309</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B55" s="5">
-        <v>96503</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="5">
-        <v>95346</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="5">
-        <v>92526</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" s="5">
-        <v>91632</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="5">
-        <v>87541</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="5">
-        <v>84304</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" s="5">
-        <v>74201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="5">
-        <v>61939</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B63" s="5">
-        <v>54102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="5">
-        <v>51225</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B65" s="5">
-        <v>45587</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="5">
-        <v>40689</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="5">
-        <v>27714</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B68" s="5">
-        <v>663452</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="5">
-        <v>90608</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B70" s="5">
-        <v>82871</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="5">
-        <v>74344</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B72" s="5">
-        <v>71398</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="5">
-        <v>62472</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" s="5">
-        <v>52320</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="5">
-        <v>50558</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B76" s="5">
-        <v>50441</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" s="5">
-        <v>36220</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B78" s="5">
-        <v>33787</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" s="5">
-        <v>32929</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B80" s="5">
-        <v>25504</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B81" s="5">
-        <v>1067110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="5">
-        <v>90328</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="5">
-        <v>89126</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="5">
-        <v>87369</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B85" s="5">
-        <v>83237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B86" s="5">
-        <v>78859</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B87" s="5">
-        <v>74903</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88" s="5">
-        <v>60066</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B89" s="5">
-        <v>56934</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B90" s="5">
-        <v>56102</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B91" s="5">
-        <v>53638</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B92" s="5">
-        <v>51651</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93" s="5">
-        <v>50945</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B94" s="5">
-        <v>47939</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B95" s="5">
-        <v>43304</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="5">
-        <v>39748</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B97" s="5">
-        <v>38413</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B98" s="5">
-        <v>37471</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B99" s="5">
-        <v>27077</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B100" s="5">
-        <v>653792</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B101" s="5">
-        <v>92006</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B102" s="5">
-        <v>91367</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B103" s="5">
-        <v>85983</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B104" s="5">
-        <v>85414</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B105" s="5">
-        <v>79169</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106" s="5">
-        <v>67560</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B107" s="5">
-        <v>62997</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B108" s="5">
-        <v>59404</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B109" s="5">
-        <v>29892</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B110" s="5">
-        <v>6325726</v>
+        <v>397828</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:B10" xr:uid="{4F8EEB18-62AF-48A5-8FC5-BF1CEC0909F8}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Aiden Oconnell"/>
+        <filter val="Alisa Davies"/>
+        <filter val="Amaris Waters"/>
+        <filter val="Anya Anderson"/>
+        <filter val="Ayanna Maldonado"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>